<commit_message>
elsa s02 GUI outline tested with empty methods.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A234BE93-BAA5-4750-8902-4B7628FCDF29}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD476A4-1CDA-41D1-959D-DA1162673543}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="160">
   <si>
     <t>Product Name:</t>
   </si>
@@ -497,9 +497,6 @@
   </si>
   <si>
     <t>Write set_* method</t>
-  </si>
-  <si>
-    <t>Finished in Sprint 2</t>
   </si>
   <si>
     <t>Write entry dialog to display in GUI</t>
@@ -1189,16 +1186,16 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1803,22 +1800,22 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3150,7 +3147,7 @@
   <dimension ref="A1:AMK95"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3384,11 +3381,11 @@
       </c>
       <c r="B14" s="2">
         <f>B13-C14</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C14" s="8">
         <f>COUNTIF(G$24:G$101,"Finished in Sprint 2")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
@@ -3408,7 +3405,7 @@
       </c>
       <c r="B15" s="2">
         <f>B14-C15</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(G$24:G$101,"Finished in Sprint 3")</f>
@@ -3432,7 +3429,7 @@
       </c>
       <c r="B16" s="2">
         <f>B15-C16</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$101,"Finished in Sprint 4")</f>
@@ -3452,7 +3449,7 @@
       </c>
       <c r="B17" s="2">
         <f>B16-C17</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$101,"Finished in Sprint 4")</f>
@@ -3758,9 +3755,7 @@
         <v>8</v>
       </c>
       <c r="F30" s="18"/>
-      <c r="G30" s="18" t="s">
-        <v>154</v>
-      </c>
+      <c r="G30" s="18"/>
       <c r="H30" s="19" t="s">
         <v>31</v>
       </c>
@@ -3789,9 +3784,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="18"/>
-      <c r="G31" s="18" t="s">
-        <v>154</v>
-      </c>
+      <c r="G31" s="18"/>
       <c r="H31" s="19" t="s">
         <v>57</v>
       </c>
@@ -6158,7 +6151,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6298,11 +6291,11 @@
       </c>
       <c r="B9" s="30">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9" s="30"/>
       <c r="E9" s="30"/>
@@ -6316,7 +6309,7 @@
       </c>
       <c r="B10" s="30">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -6334,7 +6327,7 @@
       </c>
       <c r="B11" s="30">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -6352,7 +6345,7 @@
       </c>
       <c r="B12" s="30">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -6370,7 +6363,7 @@
       </c>
       <c r="B13" s="30">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -6388,7 +6381,7 @@
       </c>
       <c r="B14" s="30">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6503,7 +6496,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E21" s="42" t="s">
         <v>150</v>
@@ -6519,7 +6512,7 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E22" s="42" t="s">
         <v>150</v>
@@ -6535,10 +6528,10 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F23" s="43"/>
     </row>
@@ -6553,7 +6546,9 @@
       <c r="D24" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="E24" s="42"/>
+      <c r="E24" s="42" t="s">
+        <v>146</v>
+      </c>
       <c r="F24" s="43"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -6565,7 +6560,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E25" s="42"/>
       <c r="F25" s="43"/>
@@ -6579,7 +6574,7 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E26" s="42"/>
       <c r="F26" s="43"/>
@@ -6593,7 +6588,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E27" s="42"/>
       <c r="F27" s="43"/>

</xml_diff>

<commit_message>
elsa s02 get methods completed along with utility.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD476A4-1CDA-41D1-959D-DA1162673543}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125D2239-3335-46F7-A989-4A70C70327FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="160">
   <si>
     <t>Product Name:</t>
   </si>
@@ -496,9 +496,6 @@
     <t>Write on_about_click method</t>
   </si>
   <si>
-    <t>Write set_* method</t>
-  </si>
-  <si>
     <t>Write entry dialog to display in GUI</t>
   </si>
   <si>
@@ -511,10 +508,13 @@
     <t>Write main.cpp to test so far</t>
   </si>
   <si>
-    <t>Write view_* methods</t>
-  </si>
-  <si>
-    <t>Write insert_* methods</t>
+    <t>Completed Day 3</t>
+  </si>
+  <si>
+    <t>write all insert methods</t>
+  </si>
+  <si>
+    <t>write all view methi</t>
   </si>
 </sst>
 </file>
@@ -1803,19 +1803,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6151,7 +6151,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6309,11 +6309,11 @@
       </c>
       <c r="B10" s="30">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -6327,7 +6327,7 @@
       </c>
       <c r="B11" s="30">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -6345,7 +6345,7 @@
       </c>
       <c r="B12" s="30">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -6363,7 +6363,7 @@
       </c>
       <c r="B13" s="30">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="B14" s="30">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6496,7 +6496,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E21" s="42" t="s">
         <v>150</v>
@@ -6512,7 +6512,7 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E22" s="42" t="s">
         <v>150</v>
@@ -6528,7 +6528,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E23" s="42" t="s">
         <v>150</v>
@@ -6544,10 +6544,10 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="41" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="F24" s="43"/>
     </row>
@@ -6560,9 +6560,11 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="41" t="s">
-        <v>155</v>
-      </c>
-      <c r="E25" s="42"/>
+        <v>158</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>146</v>
+      </c>
       <c r="F25" s="43"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -6574,7 +6576,7 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="41" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E26" s="42"/>
       <c r="F26" s="43"/>
@@ -6588,7 +6590,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="41" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E27" s="42"/>
       <c r="F27" s="43"/>

</xml_diff>

<commit_message>
elsa s02 customer insert and view method created.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125D2239-3335-46F7-A989-4A70C70327FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F23F89-E310-4D4F-B568-DF2282EFE54E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="163">
   <si>
     <t>Product Name:</t>
   </si>
@@ -511,10 +511,19 @@
     <t>Completed Day 3</t>
   </si>
   <si>
-    <t>write all insert methods</t>
-  </si>
-  <si>
-    <t>write all view methi</t>
+    <t>write insert customer method</t>
+  </si>
+  <si>
+    <t>write all view customer method</t>
+  </si>
+  <si>
+    <t>write rest of the insert methods</t>
+  </si>
+  <si>
+    <t>write the rest of the view methods</t>
+  </si>
+  <si>
+    <t>Final touch up</t>
   </si>
 </sst>
 </file>
@@ -1794,13 +1803,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
@@ -6151,7 +6160,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6258,7 +6267,7 @@
       </c>
       <c r="B7" s="30">
         <f>COUNTA(D17:D995)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
@@ -6273,7 +6282,7 @@
       </c>
       <c r="B8" s="30">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -6291,7 +6300,7 @@
       </c>
       <c r="B9" s="30">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -6313,7 +6322,7 @@
       </c>
       <c r="C10" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -6563,7 +6572,7 @@
         <v>158</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="F25" s="43"/>
     </row>
@@ -6578,7 +6587,9 @@
       <c r="D26" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="E26" s="42"/>
+      <c r="E26" s="42" t="s">
+        <v>157</v>
+      </c>
       <c r="F26" s="43"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -6590,18 +6601,24 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="E27" s="42"/>
+        <v>160</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>146</v>
+      </c>
       <c r="F27" s="43"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>12</v>
       </c>
-      <c r="B28" s="40"/>
+      <c r="B28" s="40" t="s">
+        <v>44</v>
+      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="41"/>
+      <c r="D28" s="41" t="s">
+        <v>161</v>
+      </c>
       <c r="E28" s="42"/>
       <c r="F28" s="43"/>
     </row>
@@ -6611,7 +6628,9 @@
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="41"/>
+      <c r="D29" s="41" t="s">
+        <v>162</v>
+      </c>
       <c r="E29" s="42"/>
       <c r="F29" s="43"/>
     </row>

</xml_diff>

<commit_message>
elsa s03 first phase completed.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3576E52-ABC4-4E5E-B4EB-9BF7ECCE9090}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D68B00-5BB5-4AE4-A7F3-F4DBD4618D62}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="170">
   <si>
     <t>Product Name:</t>
   </si>
@@ -533,6 +533,21 @@
   </si>
   <si>
     <t>Program completed.</t>
+  </si>
+  <si>
+    <t>Create save method and matching constructor to each class</t>
+  </si>
+  <si>
+    <t>In Work</t>
+  </si>
+  <si>
+    <t>Install I/O Framework and test</t>
+  </si>
+  <si>
+    <t>Adding dialog box to open and save file</t>
+  </si>
+  <si>
+    <t>Write call functions to dialog</t>
   </si>
 </sst>
 </file>
@@ -2350,7 +2365,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -2428,28 +2443,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2499,7 +2514,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -2573,7 +2588,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -3131,9 +3146,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>438866</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>136290</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3568,8 +3583,8 @@
   </sheetPr>
   <dimension ref="A1:AMK95"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6440,8 +6455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7683,8 +7698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7692,7 +7707,7 @@
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.5546875"/>
     <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="51.88671875" customWidth="1"/>
+    <col min="4" max="4" width="53" customWidth="1"/>
     <col min="5" max="5" width="17.77734375" customWidth="1"/>
     <col min="6" max="6" width="51.88671875" customWidth="1"/>
     <col min="7" max="1025" width="11.5546875"/>
@@ -7791,7 +7806,7 @@
       </c>
       <c r="B7" s="29">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -7806,11 +7821,11 @@
       </c>
       <c r="B8" s="29">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -7824,7 +7839,7 @@
       </c>
       <c r="B9" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -7842,7 +7857,7 @@
       </c>
       <c r="B10" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -7860,7 +7875,7 @@
       </c>
       <c r="B11" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -7878,7 +7893,7 @@
       </c>
       <c r="B12" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -7896,7 +7911,7 @@
       </c>
       <c r="B13" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -7914,7 +7929,7 @@
       </c>
       <c r="B14" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -7956,45 +7971,65 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="37"/>
+      <c r="B17" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="E17" s="39"/>
+        <v>165</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>146</v>
+      </c>
       <c r="F17" s="40"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2</v>
       </c>
-      <c r="B18" s="37"/>
+      <c r="B18" s="37" t="s">
+        <v>44</v>
+      </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
+      <c r="D18" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>146</v>
+      </c>
       <c r="F18" s="40"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>3</v>
       </c>
-      <c r="B19" s="37"/>
+      <c r="B19" s="37" t="s">
+        <v>44</v>
+      </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
+      <c r="D19" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>166</v>
+      </c>
       <c r="F19" s="40"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>4</v>
       </c>
-      <c r="B20" s="37"/>
+      <c r="B20" s="37" t="s">
+        <v>44</v>
+      </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="38"/>
+      <c r="D20" s="38" t="s">
+        <v>169</v>
+      </c>
       <c r="E20" s="39"/>
       <c r="F20" s="40"/>
     </row>
@@ -8002,7 +8037,9 @@
       <c r="A21" s="1">
         <v>5</v>
       </c>
-      <c r="B21" s="37"/>
+      <c r="B21" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="38"/>
       <c r="E21" s="39"/>

</xml_diff>

<commit_message>
elsa s03 phase 2 completed.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D68B00-5BB5-4AE4-A7F3-F4DBD4618D62}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36CE005-CE9B-454D-B05C-89C099C6E7DE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="173">
   <si>
     <t>Product Name:</t>
   </si>
@@ -548,6 +548,15 @@
   </si>
   <si>
     <t>Write call functions to dialog</t>
+  </si>
+  <si>
+    <t>Write save as function</t>
+  </si>
+  <si>
+    <t>write save functions for each classes</t>
+  </si>
+  <si>
+    <t>write load methods for each classes</t>
   </si>
 </sst>
 </file>
@@ -2443,10 +2452,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
@@ -3146,9 +3155,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>438866</xdr:colOff>
+      <xdr:colOff>435056</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>136290</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7699,7 +7708,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7806,7 +7815,7 @@
       </c>
       <c r="B7" s="29">
         <f>COUNTA(D17:D995)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -7821,7 +7830,7 @@
       </c>
       <c r="B8" s="29">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -7843,7 +7852,7 @@
       </c>
       <c r="C9" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
@@ -8015,7 +8024,7 @@
         <v>168</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="F19" s="40"/>
     </row>
@@ -8030,7 +8039,9 @@
       <c r="D20" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="E20" s="39"/>
+      <c r="E20" s="39" t="s">
+        <v>149</v>
+      </c>
       <c r="F20" s="40"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -8038,30 +8049,44 @@
         <v>5</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
+      <c r="D21" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>149</v>
+      </c>
       <c r="F21" s="40"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>6</v>
       </c>
-      <c r="B22" s="37"/>
+      <c r="B22" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
+      <c r="D22" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>166</v>
+      </c>
       <c r="F22" s="40"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>7</v>
       </c>
-      <c r="B23" s="37"/>
+      <c r="B23" s="37" t="s">
+        <v>68</v>
+      </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="38"/>
+      <c r="D23" s="38" t="s">
+        <v>172</v>
+      </c>
       <c r="E23" s="39"/>
       <c r="F23" s="40"/>
     </row>

</xml_diff>

<commit_message>
elsa s03 save method for customer .
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36CE005-CE9B-454D-B05C-89C099C6E7DE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3428488-8FA5-42A1-BC30-30C1857484CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="179">
   <si>
     <t>Product Name:</t>
   </si>
@@ -553,10 +553,28 @@
     <t>Write save as function</t>
   </si>
   <si>
-    <t>write save functions for each classes</t>
-  </si>
-  <si>
-    <t>write load methods for each classes</t>
+    <t>write save functions for customer class</t>
+  </si>
+  <si>
+    <t>write load methods for customer class</t>
+  </si>
+  <si>
+    <t>write save functions for options class</t>
+  </si>
+  <si>
+    <t>write save functions for desktop class</t>
+  </si>
+  <si>
+    <t>write save functions for order class</t>
+  </si>
+  <si>
+    <t>write load methods for option class</t>
+  </si>
+  <si>
+    <t>write load methods for desktop class</t>
+  </si>
+  <si>
+    <t>write load methods for order class</t>
   </si>
 </sst>
 </file>
@@ -2452,28 +2470,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3593,7 +3611,7 @@
   <dimension ref="A1:AMK95"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7707,8 +7725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7815,7 +7833,7 @@
       </c>
       <c r="B7" s="29">
         <f>COUNTA(D17:D995)</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -7830,7 +7848,7 @@
       </c>
       <c r="B8" s="29">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C8" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -7848,11 +7866,11 @@
       </c>
       <c r="B9" s="29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C9" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
@@ -7866,7 +7884,7 @@
       </c>
       <c r="B10" s="29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C10" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -7884,7 +7902,7 @@
       </c>
       <c r="B11" s="29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C11" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -7902,7 +7920,7 @@
       </c>
       <c r="B12" s="29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C12" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -7920,7 +7938,7 @@
       </c>
       <c r="B13" s="29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C13" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -7938,7 +7956,7 @@
       </c>
       <c r="B14" s="29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C14" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -8072,7 +8090,7 @@
         <v>171</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="F22" s="40"/>
     </row>
@@ -8087,26 +8105,38 @@
       <c r="D23" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="E23" s="39"/>
+      <c r="E23" s="39" t="s">
+        <v>149</v>
+      </c>
       <c r="F23" s="40"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>8</v>
       </c>
-      <c r="B24" s="37"/>
+      <c r="B24" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="39"/>
+      <c r="D24" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>166</v>
+      </c>
       <c r="F24" s="40"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>9</v>
       </c>
-      <c r="B25" s="37"/>
+      <c r="B25" s="37" t="s">
+        <v>68</v>
+      </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="38"/>
+      <c r="D25" s="38" t="s">
+        <v>176</v>
+      </c>
       <c r="E25" s="39"/>
       <c r="F25" s="40"/>
     </row>
@@ -8114,9 +8144,13 @@
       <c r="A26" s="1">
         <v>10</v>
       </c>
-      <c r="B26" s="37"/>
+      <c r="B26" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="38"/>
+      <c r="D26" s="38" t="s">
+        <v>174</v>
+      </c>
       <c r="E26" s="39"/>
       <c r="F26" s="40"/>
     </row>
@@ -8124,9 +8158,13 @@
       <c r="A27" s="1">
         <v>11</v>
       </c>
-      <c r="B27" s="37"/>
+      <c r="B27" s="37" t="s">
+        <v>68</v>
+      </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="38"/>
+      <c r="D27" s="38" t="s">
+        <v>177</v>
+      </c>
       <c r="E27" s="39"/>
       <c r="F27" s="40"/>
     </row>
@@ -8134,9 +8172,13 @@
       <c r="A28" s="1">
         <v>12</v>
       </c>
-      <c r="B28" s="37"/>
+      <c r="B28" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="38"/>
+      <c r="D28" s="38" t="s">
+        <v>175</v>
+      </c>
       <c r="E28" s="39"/>
       <c r="F28" s="40"/>
     </row>
@@ -8144,9 +8186,13 @@
       <c r="A29" s="1">
         <v>13</v>
       </c>
-      <c r="B29" s="37"/>
+      <c r="B29" s="37" t="s">
+        <v>68</v>
+      </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="38"/>
+      <c r="D29" s="38" t="s">
+        <v>178</v>
+      </c>
       <c r="E29" s="39"/>
       <c r="F29" s="40"/>
     </row>

</xml_diff>

<commit_message>
elsa s03 save and load for dekstop.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3428488-8FA5-42A1-BC30-30C1857484CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F56C15-0046-432F-B23E-6FFA0EAEEB1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="180">
   <si>
     <t>Product Name:</t>
   </si>
@@ -575,6 +575,9 @@
   </si>
   <si>
     <t>write load methods for order class</t>
+  </si>
+  <si>
+    <t>testing error</t>
   </si>
 </sst>
 </file>
@@ -2470,28 +2473,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3610,8 +3613,8 @@
   </sheetPr>
   <dimension ref="A1:AMK95"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4281,7 +4284,9 @@
         <v>13</v>
       </c>
       <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="G32" s="18" t="s">
+        <v>166</v>
+      </c>
       <c r="H32" s="19" t="s">
         <v>61</v>
       </c>
@@ -4310,7 +4315,9 @@
         <v>5</v>
       </c>
       <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="G33" s="18" t="s">
+        <v>166</v>
+      </c>
       <c r="H33" s="19" t="s">
         <v>61</v>
       </c>
@@ -4339,7 +4346,9 @@
         <v>8</v>
       </c>
       <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="G34" s="18" t="s">
+        <v>166</v>
+      </c>
       <c r="H34" s="19" t="s">
         <v>61</v>
       </c>
@@ -7725,8 +7734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7833,7 +7842,7 @@
       </c>
       <c r="B7" s="29">
         <f>COUNTA(D17:D995)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -7848,7 +7857,7 @@
       </c>
       <c r="B8" s="29">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -7866,11 +7875,11 @@
       </c>
       <c r="B9" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C9" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
@@ -7884,7 +7893,7 @@
       </c>
       <c r="B10" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C10" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -7902,7 +7911,7 @@
       </c>
       <c r="B11" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C11" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -7920,7 +7929,7 @@
       </c>
       <c r="B12" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -7938,7 +7947,7 @@
       </c>
       <c r="B13" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C13" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -7956,7 +7965,7 @@
       </c>
       <c r="B14" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -8122,7 +8131,7 @@
         <v>173</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="F24" s="40"/>
     </row>
@@ -8137,7 +8146,9 @@
       <c r="D25" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="E25" s="39"/>
+      <c r="E25" s="39" t="s">
+        <v>149</v>
+      </c>
       <c r="F25" s="40"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -8151,7 +8162,9 @@
       <c r="D26" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="E26" s="39"/>
+      <c r="E26" s="39" t="s">
+        <v>149</v>
+      </c>
       <c r="F26" s="40"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -8165,7 +8178,9 @@
       <c r="D27" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="E27" s="39"/>
+      <c r="E27" s="39" t="s">
+        <v>149</v>
+      </c>
       <c r="F27" s="40"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -8179,7 +8194,9 @@
       <c r="D28" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="E28" s="39"/>
+      <c r="E28" s="39" t="s">
+        <v>166</v>
+      </c>
       <c r="F28" s="40"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -8193,7 +8210,9 @@
       <c r="D29" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="E29" s="39"/>
+      <c r="E29" s="39" t="s">
+        <v>166</v>
+      </c>
       <c r="F29" s="40"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -8202,7 +8221,9 @@
       </c>
       <c r="B30" s="37"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="38"/>
+      <c r="D30" s="38" t="s">
+        <v>179</v>
+      </c>
       <c r="E30" s="39"/>
       <c r="F30" s="40"/>
     </row>

</xml_diff>

<commit_message>
elsa s03 program completed.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F56C15-0046-432F-B23E-6FFA0EAEEB1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51A537D-4D3D-4F77-8C3D-712BD3FA12CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="180">
   <si>
     <t>Product Name:</t>
   </si>
@@ -2482,19 +2482,19 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7735,7 +7735,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7893,11 +7893,11 @@
       </c>
       <c r="B10" s="29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
@@ -7911,7 +7911,7 @@
       </c>
       <c r="B11" s="29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -7929,7 +7929,7 @@
       </c>
       <c r="B12" s="29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -7947,7 +7947,7 @@
       </c>
       <c r="B13" s="29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -7965,7 +7965,7 @@
       </c>
       <c r="B14" s="29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -8195,7 +8195,7 @@
         <v>175</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="F28" s="40"/>
     </row>
@@ -8211,7 +8211,7 @@
         <v>178</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="F29" s="40"/>
     </row>
@@ -8224,7 +8224,9 @@
       <c r="D30" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="E30" s="39"/>
+      <c r="E30" s="39" t="s">
+        <v>166</v>
+      </c>
       <c r="F30" s="40"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
elsa s03 completed and tested.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51A537D-4D3D-4F77-8C3D-712BD3FA12CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205F8DF3-868F-4D2D-8249-BF42C29B3C58}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -538,9 +538,6 @@
     <t>Create save method and matching constructor to each class</t>
   </si>
   <si>
-    <t>In Work</t>
-  </si>
-  <si>
     <t>Install I/O Framework and test</t>
   </si>
   <si>
@@ -578,6 +575,9 @@
   </si>
   <si>
     <t>testing error</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 3</t>
   </si>
 </sst>
 </file>
@@ -1247,13 +1247,13 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2482,19 +2482,19 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3613,8 +3613,8 @@
   </sheetPr>
   <dimension ref="A1:AMK95"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3872,11 +3872,11 @@
       </c>
       <c r="B15" s="2">
         <f>B14-C15</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(G$24:G$101,"Finished in Sprint 3")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
@@ -3896,7 +3896,7 @@
       </c>
       <c r="B16" s="2">
         <f>B15-C16</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$101,"Finished in Sprint 4")</f>
@@ -3916,7 +3916,7 @@
       </c>
       <c r="B17" s="2">
         <f>B16-C17</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$101,"Finished in Sprint 4")</f>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="F32" s="18"/>
       <c r="G32" s="18" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="H32" s="19" t="s">
         <v>61</v>
@@ -4316,7 +4316,7 @@
       </c>
       <c r="F33" s="18"/>
       <c r="G33" s="18" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="H33" s="19" t="s">
         <v>61</v>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="18" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="H34" s="19" t="s">
         <v>61</v>
@@ -7734,8 +7734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7893,11 +7893,11 @@
       </c>
       <c r="B10" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
@@ -7911,7 +7911,7 @@
       </c>
       <c r="B11" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -7929,7 +7929,7 @@
       </c>
       <c r="B12" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -7947,7 +7947,7 @@
       </c>
       <c r="B13" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -7965,7 +7965,7 @@
       </c>
       <c r="B14" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -8032,7 +8032,7 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E18" s="39" t="s">
         <v>146</v>
@@ -8048,7 +8048,7 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E19" s="39" t="s">
         <v>149</v>
@@ -8064,7 +8064,7 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E20" s="39" t="s">
         <v>149</v>
@@ -8080,7 +8080,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E21" s="39" t="s">
         <v>149</v>
@@ -8096,7 +8096,7 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E22" s="39" t="s">
         <v>149</v>
@@ -8112,7 +8112,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="38" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E23" s="39" t="s">
         <v>149</v>
@@ -8128,7 +8128,7 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E24" s="39" t="s">
         <v>149</v>
@@ -8144,7 +8144,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E25" s="39" t="s">
         <v>149</v>
@@ -8160,7 +8160,7 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E26" s="39" t="s">
         <v>149</v>
@@ -8176,7 +8176,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E27" s="39" t="s">
         <v>149</v>
@@ -8192,7 +8192,7 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E28" s="39" t="s">
         <v>156</v>
@@ -8208,7 +8208,7 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E29" s="39" t="s">
         <v>156</v>
@@ -8222,10 +8222,10 @@
       <c r="B30" s="37"/>
       <c r="C30" s="1"/>
       <c r="D30" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="F30" s="40"/>
     </row>

</xml_diff>

<commit_message>
elsa s04 first item modify.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205F8DF3-868F-4D2D-8249-BF42C29B3C58}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12434935-C9E9-4708-AB98-D4DFE0BFD777}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="182">
   <si>
     <t>Product Name:</t>
   </si>
@@ -463,9 +463,6 @@
     <t>Ensure ALL CODE is on GitHub by deadline!</t>
   </si>
   <si>
-    <t>--&gt; Add tasks to complete each feature for this sprint</t>
-  </si>
-  <si>
     <t>Night Coder</t>
   </si>
   <si>
@@ -578,6 +575,15 @@
   </si>
   <si>
     <t>Finished in Sprint 3</t>
+  </si>
+  <si>
+    <t>In Test</t>
+  </si>
+  <si>
+    <t>Replacing customer insertion dialog</t>
+  </si>
+  <si>
+    <t>In Work</t>
   </si>
 </sst>
 </file>
@@ -2709,7 +2715,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -2858,7 +2864,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -2932,7 +2938,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -3613,8 +3619,8 @@
   </sheetPr>
   <dimension ref="A1:AMK95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3656,7 +3662,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -3702,7 +3708,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
@@ -3710,7 +3716,7 @@
       <c r="F5" s="47"/>
       <c r="G5" s="47"/>
       <c r="H5" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I5" s="42">
         <v>1001520302</v>
@@ -4047,7 +4053,7 @@
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H24" s="19" t="s">
         <v>31</v>
@@ -4076,7 +4082,7 @@
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H25" s="19" t="s">
         <v>35</v>
@@ -4105,7 +4111,7 @@
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H26" s="19" t="s">
         <v>31</v>
@@ -4134,7 +4140,7 @@
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H27" s="19" t="s">
         <v>31</v>
@@ -4163,7 +4169,7 @@
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H28" s="19" t="s">
         <v>31</v>
@@ -4194,7 +4200,7 @@
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H29" s="19" t="s">
         <v>31</v>
@@ -4225,7 +4231,7 @@
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H30" s="19" t="s">
         <v>31</v>
@@ -4256,7 +4262,7 @@
       </c>
       <c r="F31" s="18"/>
       <c r="G31" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H31" s="19" t="s">
         <v>57</v>
@@ -4285,7 +4291,7 @@
       </c>
       <c r="F32" s="18"/>
       <c r="G32" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H32" s="19" t="s">
         <v>61</v>
@@ -4316,7 +4322,7 @@
       </c>
       <c r="F33" s="18"/>
       <c r="G33" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H33" s="19" t="s">
         <v>61</v>
@@ -4347,7 +4353,7 @@
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H34" s="19" t="s">
         <v>61</v>
@@ -4404,7 +4410,9 @@
         <v>8</v>
       </c>
       <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="G36" s="18" t="s">
+        <v>179</v>
+      </c>
       <c r="H36" s="19" t="s">
         <v>31</v>
       </c>
@@ -5676,7 +5684,7 @@
         <v>122</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F17" t="s">
         <v>123</v>
@@ -5693,7 +5701,7 @@
         <v>124</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F18" t="s">
         <v>125</v>
@@ -5710,7 +5718,7 @@
         <v>126</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -5724,7 +5732,7 @@
         <v>128</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -5738,7 +5746,7 @@
         <v>129</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -5752,7 +5760,7 @@
         <v>130</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -5766,7 +5774,7 @@
         <v>131</v>
       </c>
       <c r="E23" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -5780,7 +5788,7 @@
         <v>132</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -5794,7 +5802,7 @@
         <v>133</v>
       </c>
       <c r="E25" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -5808,7 +5816,7 @@
         <v>134</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -5822,7 +5830,7 @@
         <v>135</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -5836,7 +5844,7 @@
         <v>136</v>
       </c>
       <c r="E28" s="44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -5850,7 +5858,7 @@
         <v>137</v>
       </c>
       <c r="E29" s="44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -5864,7 +5872,7 @@
         <v>138</v>
       </c>
       <c r="E30" s="44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -5878,7 +5886,7 @@
         <v>139</v>
       </c>
       <c r="E31" s="44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -5892,7 +5900,7 @@
         <v>140</v>
       </c>
       <c r="E32" s="44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -6773,10 +6781,10 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F17" s="40"/>
     </row>
@@ -6789,10 +6797,10 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F18" s="40"/>
     </row>
@@ -6805,10 +6813,10 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F19" s="40"/>
     </row>
@@ -6821,10 +6829,10 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F20" s="40"/>
     </row>
@@ -6837,10 +6845,10 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F21" s="40"/>
     </row>
@@ -6853,10 +6861,10 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F22" s="40"/>
     </row>
@@ -6869,10 +6877,10 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F23" s="40"/>
     </row>
@@ -6885,10 +6893,10 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F24" s="40"/>
     </row>
@@ -6901,10 +6909,10 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F25" s="40"/>
     </row>
@@ -6917,10 +6925,10 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E26" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F26" s="40"/>
     </row>
@@ -6933,10 +6941,10 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E27" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F27" s="40"/>
     </row>
@@ -6949,10 +6957,10 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F28" s="40"/>
     </row>
@@ -6963,13 +6971,13 @@
       <c r="B29" s="37"/>
       <c r="C29" s="1"/>
       <c r="D29" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="E29" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="E29" s="39" t="s">
-        <v>162</v>
-      </c>
       <c r="F29" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -8016,10 +8024,10 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F17" s="40"/>
     </row>
@@ -8032,10 +8040,10 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F18" s="40"/>
     </row>
@@ -8048,10 +8056,10 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F19" s="40"/>
     </row>
@@ -8064,10 +8072,10 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F20" s="40"/>
     </row>
@@ -8080,10 +8088,10 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F21" s="40"/>
     </row>
@@ -8096,10 +8104,10 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F22" s="40"/>
     </row>
@@ -8112,10 +8120,10 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E23" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F23" s="40"/>
     </row>
@@ -8128,10 +8136,10 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="38" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F24" s="40"/>
     </row>
@@ -8144,10 +8152,10 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F25" s="40"/>
     </row>
@@ -8160,10 +8168,10 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E26" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F26" s="40"/>
     </row>
@@ -8176,10 +8184,10 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E27" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F27" s="40"/>
     </row>
@@ -8192,10 +8200,10 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F28" s="40"/>
     </row>
@@ -8208,10 +8216,10 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F29" s="40"/>
     </row>
@@ -8222,10 +8230,10 @@
       <c r="B30" s="37"/>
       <c r="C30" s="1"/>
       <c r="D30" s="38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F30" s="40"/>
     </row>
@@ -8981,8 +8989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9258,12 +9266,16 @@
       <c r="A17" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="37"/>
+      <c r="B17" s="37" t="s">
+        <v>74</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="E17" s="39"/>
+        <v>180</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>181</v>
+      </c>
       <c r="F17" s="40" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
elsa s04 working on ram opt.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
+++ b/elsa/doc/Scrum_ELSA_Sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12434935-C9E9-4708-AB98-D4DFE0BFD777}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7723D8D-052F-4E7A-9D78-15EF803C9684}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="183">
   <si>
     <t>Product Name:</t>
   </si>
@@ -577,13 +577,16 @@
     <t>Finished in Sprint 3</t>
   </si>
   <si>
-    <t>In Test</t>
-  </si>
-  <si>
     <t>Replacing customer insertion dialog</t>
   </si>
   <si>
     <t>In Work</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 4</t>
+  </si>
+  <si>
+    <t>creating new option for peripherals</t>
   </si>
 </sst>
 </file>
@@ -1256,10 +1259,10 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2793,7 +2796,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -3620,7 +3623,7 @@
   <dimension ref="A1:AMK95"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3902,11 +3905,11 @@
       </c>
       <c r="B16" s="2">
         <f>B15-C16</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$101,"Finished in Sprint 4")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
@@ -3922,11 +3925,11 @@
       </c>
       <c r="B17" s="2">
         <f>B16-C17</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$101,"Finished in Sprint 4")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
@@ -4383,7 +4386,9 @@
         <v>21</v>
       </c>
       <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="G35" s="18" t="s">
+        <v>180</v>
+      </c>
       <c r="H35" s="19" t="s">
         <v>71</v>
       </c>
@@ -4411,7 +4416,7 @@
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="18" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H36" s="19" t="s">
         <v>31</v>
@@ -8990,7 +8995,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9097,7 +9102,7 @@
       </c>
       <c r="B7" s="29">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -9116,7 +9121,7 @@
       </c>
       <c r="C8" s="29">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -9271,10 +9276,10 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="F17" s="40" t="s">
         <v>127</v>
@@ -9284,10 +9289,16 @@
       <c r="A18" s="1">
         <v>2</v>
       </c>
-      <c r="B18" s="37"/>
+      <c r="B18" s="37" t="s">
+        <v>70</v>
+      </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
+      <c r="D18" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>180</v>
+      </c>
       <c r="F18" s="40"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>